<commit_message>
add Account Creation test class
</commit_message>
<xml_diff>
--- a/src/main/resource/testdata/OpenCartRegUserTestData.xlsx
+++ b/src/main/resource/testdata/OpenCartRegUserTestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SELENIUM_POM_OPENCART_PRACTISE\Jan2023_OpenCart_Practise\src\main\resource\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MY_Selenium_POM\src\main\resource\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C70901-1B73-4E67-846F-56F227F7A046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FFCABD-B4F4-4358-87DF-33DBA0688251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{7B1AA3E2-B494-4213-8E38-6CBE51FC50B4}"/>
   </bookViews>
@@ -36,63 +36,72 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
-  <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>telephone</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>subscribe</t>
-  </si>
-  <si>
-    <t>abhi</t>
-  </si>
-  <si>
-    <t>anand</t>
-  </si>
-  <si>
-    <t>abhi@123</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>robinson</t>
-  </si>
-  <si>
-    <t>matinez</t>
-  </si>
-  <si>
-    <t>robin@123</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>amber</t>
-  </si>
-  <si>
-    <t>automation</t>
-  </si>
-  <si>
-    <t>amber@123</t>
-  </si>
-  <si>
-    <t>9898989898</t>
-  </si>
-  <si>
-    <t>8976098765</t>
-  </si>
-  <si>
-    <t>7654321098</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+  <si>
+    <t>Account Name</t>
+  </si>
+  <si>
+    <t>Account Number</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Shipping Street_c</t>
+  </si>
+  <si>
+    <t>Shipping State_c</t>
+  </si>
+  <si>
+    <t>Shipping City_c</t>
+  </si>
+  <si>
+    <t>Shipping Country_c</t>
+  </si>
+  <si>
+    <t>Shipping Zipcode_c</t>
+  </si>
+  <si>
+    <t>Test_Automation_Account</t>
+  </si>
+  <si>
+    <t>TAACC-001</t>
+  </si>
+  <si>
+    <t>This Account is created By Selenium Automation Script</t>
+  </si>
+  <si>
+    <t>2101 West Vineyard Avenue</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Oxnard</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>TestName</t>
+  </si>
+  <si>
+    <t>Creating New Account</t>
+  </si>
+  <si>
+    <t>Editing Account</t>
+  </si>
+  <si>
+    <t>ParameterCount</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -110,15 +119,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -134,7 +142,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -162,19 +170,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -507,94 +513,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D41DAC7C-D34E-4D5E-987A-8E1EB0CBFB48}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.90625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="22.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="2">
+        <v>93030</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="B4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="E4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="2">
+        <v>93030</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{902F3B4E-74AD-4FD2-82A5-89F39521D337}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{0EB4B145-86EB-45ED-A83E-0E5C6088A591}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{097F2182-32E5-49CA-A59E-4A9771FFEAE0}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Account Creation Test
</commit_message>
<xml_diff>
--- a/src/main/resource/testdata/OpenCartRegUserTestData.xlsx
+++ b/src/main/resource/testdata/OpenCartRegUserTestData.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MY_Selenium_POM\src\main\resource\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FFCABD-B4F4-4358-87DF-33DBA0688251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0DAF6B-F4C6-4B94-8CA0-02BF52D805C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{7B1AA3E2-B494-4213-8E38-6CBE51FC50B4}"/>
+    <workbookView xWindow="4800" yWindow="1620" windowWidth="14400" windowHeight="8170" xr2:uid="{7B1AA3E2-B494-4213-8E38-6CBE51FC50B4}"/>
   </bookViews>
   <sheets>
-    <sheet name="regData" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -516,7 +516,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added Account Scenario Tests
</commit_message>
<xml_diff>
--- a/src/main/resource/testdata/OpenCartRegUserTestData.xlsx
+++ b/src/main/resource/testdata/OpenCartRegUserTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MY_Selenium_POM\src\main\resource\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0DAF6B-F4C6-4B94-8CA0-02BF52D805C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF57588-FF4F-4508-9815-1DEF51A26083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="1620" windowWidth="14400" windowHeight="8170" xr2:uid="{7B1AA3E2-B494-4213-8E38-6CBE51FC50B4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{7B1AA3E2-B494-4213-8E38-6CBE51FC50B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>Account Name</t>
   </si>
@@ -102,6 +102,18 @@
   </si>
   <si>
     <t>5</t>
+  </si>
+  <si>
+    <t>SLA Serial number</t>
+  </si>
+  <si>
+    <t>Number Of Loctions</t>
+  </si>
+  <si>
+    <t>Editing Account By Clicking Inline Btn</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -513,18 +525,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D41DAC7C-D34E-4D5E-987A-8E1EB0CBFB48}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.7265625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.90625" style="3" customWidth="1"/>
     <col min="3" max="3" width="22.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="45.1796875" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.26953125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.36328125" style="3" bestFit="1" customWidth="1"/>
@@ -646,6 +658,40 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2">
+        <v>33456</v>
+      </c>
+      <c r="D6" s="2">
+        <v>20</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>